<commit_message>
Publication des derniers chapitres
</commit_message>
<xml_diff>
--- a/dataset/pokemon.xlsx
+++ b/dataset/pokemon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Perso\IUT\cours\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anthony.sardellitti\Programmation_Statistique_R\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF81CC2-D8C8-4F35-8E8F-41DCCAF2AB57}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71435162-F681-4774-962F-F62C9046F29E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">pokemon!$A$1:$J$252</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
 </workbook>
 </file>
 
@@ -68,9 +69,6 @@
     <t>Florizarre</t>
   </si>
   <si>
-    <t>Salamèche</t>
-  </si>
-  <si>
     <t>fire</t>
   </si>
   <si>
@@ -176,15 +174,9 @@
     <t>Nidoking</t>
   </si>
   <si>
-    <t>Mélofée</t>
-  </si>
-  <si>
     <t>fairy</t>
   </si>
   <si>
-    <t>Mélodelfe</t>
-  </si>
-  <si>
     <t>Goupix</t>
   </si>
   <si>
@@ -221,9 +213,6 @@
     <t>Mimitoss</t>
   </si>
   <si>
-    <t>Aéromite</t>
-  </si>
-  <si>
     <t>Taupiqueur</t>
   </si>
   <si>
@@ -242,9 +231,6 @@
     <t>Akwakwak</t>
   </si>
   <si>
-    <t>Férosinge</t>
-  </si>
-  <si>
     <t>fighting</t>
   </si>
   <si>
@@ -260,9 +246,6 @@
     <t>Ptitard</t>
   </si>
   <si>
-    <t>Têtarte</t>
-  </si>
-  <si>
     <t>Tartard</t>
   </si>
   <si>
@@ -287,9 +270,6 @@
     <t>Mackogneur</t>
   </si>
   <si>
-    <t>Chétiflor</t>
-  </si>
-  <si>
     <t>Boustiflor</t>
   </si>
   <si>
@@ -326,12 +306,6 @@
     <t>Flagadoss</t>
   </si>
   <si>
-    <t>Magnéti</t>
-  </si>
-  <si>
-    <t>Magnéton</t>
-  </si>
-  <si>
     <t>Canarticho</t>
   </si>
   <si>
@@ -389,9 +363,6 @@
     <t>Voltorbe</t>
   </si>
   <si>
-    <t>Électrode</t>
-  </si>
-  <si>
     <t>Noeunoeuf</t>
   </si>
   <si>
@@ -422,9 +393,6 @@
     <t>Rhinocorne</t>
   </si>
   <si>
-    <t>Rhinoféros</t>
-  </si>
-  <si>
     <t>Leveinard</t>
   </si>
   <si>
@@ -437,12 +405,6 @@
     <t>Hypotrempe</t>
   </si>
   <si>
-    <t>Hypocéan</t>
-  </si>
-  <si>
-    <t>Poissirène</t>
-  </si>
-  <si>
     <t>Poissoroy</t>
   </si>
   <si>
@@ -455,18 +417,12 @@
     <t>M. Mime</t>
   </si>
   <si>
-    <t>Insécateur</t>
-  </si>
-  <si>
     <t>Lippoutou</t>
   </si>
   <si>
     <t>ice</t>
   </si>
   <si>
-    <t>Élektek</t>
-  </si>
-  <si>
     <t>Magmar</t>
   </si>
   <si>
@@ -479,18 +435,9 @@
     <t>Magicarpe</t>
   </si>
   <si>
-    <t>Léviator</t>
-  </si>
-  <si>
     <t>Lokhlass</t>
   </si>
   <si>
-    <t>Métamorph</t>
-  </si>
-  <si>
-    <t>Évoli</t>
-  </si>
-  <si>
     <t>Aquali</t>
   </si>
   <si>
@@ -515,9 +462,6 @@
     <t>Kabutops</t>
   </si>
   <si>
-    <t>Ptéra</t>
-  </si>
-  <si>
     <t>Ronflex</t>
   </si>
   <si>
@@ -527,9 +471,6 @@
     <t>Oui</t>
   </si>
   <si>
-    <t>Électhor</t>
-  </si>
-  <si>
     <t>Sulfura</t>
   </si>
   <si>
@@ -557,12 +498,6 @@
     <t>Macronium</t>
   </si>
   <si>
-    <t>Méganium</t>
-  </si>
-  <si>
-    <t>Héricendre</t>
-  </si>
-  <si>
     <t>Feurisson</t>
   </si>
   <si>
@@ -614,9 +549,6 @@
     <t>Pichu</t>
   </si>
   <si>
-    <t>Mélo</t>
-  </si>
-  <si>
     <t>Toudoudou</t>
   </si>
   <si>
@@ -671,9 +603,6 @@
     <t>Tournegrin</t>
   </si>
   <si>
-    <t>Héliatronc</t>
-  </si>
-  <si>
     <t>Yanma</t>
   </si>
   <si>
@@ -692,21 +621,12 @@
     <t>dark</t>
   </si>
   <si>
-    <t>Cornèbre</t>
-  </si>
-  <si>
     <t>Roigada</t>
   </si>
   <si>
-    <t>Feuforêve</t>
-  </si>
-  <si>
     <t>Zarbi</t>
   </si>
   <si>
-    <t>Qulbutoké</t>
-  </si>
-  <si>
     <t>Girafarig</t>
   </si>
   <si>
@@ -770,27 +690,18 @@
     <t>Corayon</t>
   </si>
   <si>
-    <t>Rémoraid</t>
-  </si>
-  <si>
     <t>Octillery</t>
   </si>
   <si>
     <t>Cadoizo</t>
   </si>
   <si>
-    <t>Démanta</t>
-  </si>
-  <si>
     <t>Airmure</t>
   </si>
   <si>
     <t>Malosse</t>
   </si>
   <si>
-    <t>Démolosse</t>
-  </si>
-  <si>
     <t>Hyporoi</t>
   </si>
   <si>
@@ -818,15 +729,9 @@
     <t>Lippouti</t>
   </si>
   <si>
-    <t>Élekid</t>
-  </si>
-  <si>
     <t>Magby</t>
   </si>
   <si>
-    <t>Écrémeuh</t>
-  </si>
-  <si>
     <t>Leuphorie</t>
   </si>
   <si>
@@ -864,6 +769,102 @@
   </si>
   <si>
     <t>Nidoqueen femelle</t>
+  </si>
+  <si>
+    <t>Melofee</t>
+  </si>
+  <si>
+    <t>Melodelfe</t>
+  </si>
+  <si>
+    <t>Aeromite</t>
+  </si>
+  <si>
+    <t>Ferosinge</t>
+  </si>
+  <si>
+    <t>Chetiflor</t>
+  </si>
+  <si>
+    <t>Magneti</t>
+  </si>
+  <si>
+    <t>Magneton</t>
+  </si>
+  <si>
+    <t>electrode</t>
+  </si>
+  <si>
+    <t>Rhinoferos</t>
+  </si>
+  <si>
+    <t>Hypocean</t>
+  </si>
+  <si>
+    <t>Insecateur</t>
+  </si>
+  <si>
+    <t>elektek</t>
+  </si>
+  <si>
+    <t>Leviator</t>
+  </si>
+  <si>
+    <t>Metamorph</t>
+  </si>
+  <si>
+    <t>evoli</t>
+  </si>
+  <si>
+    <t>Ptera</t>
+  </si>
+  <si>
+    <t>electhor</t>
+  </si>
+  <si>
+    <t>Meganium</t>
+  </si>
+  <si>
+    <t>Hericendre</t>
+  </si>
+  <si>
+    <t>Melo</t>
+  </si>
+  <si>
+    <t>Heliatronc</t>
+  </si>
+  <si>
+    <t>Qulbutoke</t>
+  </si>
+  <si>
+    <t>Remoraid</t>
+  </si>
+  <si>
+    <t>Demanta</t>
+  </si>
+  <si>
+    <t>Demolosse</t>
+  </si>
+  <si>
+    <t>elekid</t>
+  </si>
+  <si>
+    <t>ecremeuh</t>
+  </si>
+  <si>
+    <t>Salameche</t>
+  </si>
+  <si>
+    <t>Poissirene</t>
+  </si>
+  <si>
+    <t>Cornebre</t>
+  </si>
+  <si>
+    <t>Tetarte</t>
+  </si>
+  <si>
+    <t>Feuforeve</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1741,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1859,16 +1860,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
       <c r="F5">
         <v>8.5</v>
@@ -1891,7 +1892,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1900,7 +1901,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>19</v>
@@ -1923,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1932,7 +1933,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>90.5</v>
@@ -1955,16 +1956,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
       </c>
       <c r="F8">
         <v>9</v>
@@ -1987,7 +1988,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1996,7 +1997,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>22.5</v>
@@ -2019,7 +2020,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2028,7 +2029,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <v>85.5</v>
@@ -2051,16 +2052,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
       </c>
       <c r="F11">
         <v>2.9</v>
@@ -2083,7 +2084,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2092,7 +2093,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <v>9.9</v>
@@ -2115,7 +2116,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2124,7 +2125,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>32</v>
@@ -2147,7 +2148,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2156,7 +2157,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14">
         <v>3.2</v>
@@ -2179,7 +2180,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2188,7 +2189,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -2211,7 +2212,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2220,7 +2221,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16">
         <v>29.5</v>
@@ -2243,16 +2244,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
         <v>29</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
       </c>
       <c r="F17">
         <v>1.8</v>
@@ -2275,7 +2276,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2284,7 +2285,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18">
         <v>30</v>
@@ -2307,7 +2308,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2316,7 +2317,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19">
         <v>39.5</v>
@@ -2339,7 +2340,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2348,7 +2349,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20">
         <v>56</v>
@@ -2365,7 +2366,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2374,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21">
         <v>71</v>
@@ -2391,7 +2392,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2400,7 +2401,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -2423,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2432,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23">
         <v>38</v>
@@ -2455,16 +2456,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
         <v>37</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>38</v>
       </c>
       <c r="F24">
         <v>6.9</v>
@@ -2487,7 +2488,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2496,7 +2497,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25">
         <v>65</v>
@@ -2519,16 +2520,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
         <v>40</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>41</v>
       </c>
       <c r="F26">
         <v>6</v>
@@ -2551,7 +2552,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2560,7 +2561,7 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27">
         <v>85</v>
@@ -2577,16 +2578,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
         <v>43</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" t="s">
-        <v>44</v>
       </c>
       <c r="H28">
         <v>75</v>
@@ -2603,7 +2604,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2612,7 +2613,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29">
         <v>100</v>
@@ -2629,7 +2630,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2638,7 +2639,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30">
         <v>7</v>
@@ -2661,7 +2662,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2670,7 +2671,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F31">
         <v>20</v>
@@ -2693,7 +2694,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2702,7 +2703,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F32">
         <v>60</v>
@@ -2725,7 +2726,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2734,7 +2735,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F33">
         <v>9</v>
@@ -2757,7 +2758,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2766,7 +2767,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34">
         <v>19.5</v>
@@ -2789,7 +2790,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2798,7 +2799,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35">
         <v>62</v>
@@ -2821,7 +2822,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>248</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2830,7 +2831,7 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F36">
         <v>7.5</v>
@@ -2853,7 +2854,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>249</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2862,7 +2863,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F37">
         <v>40</v>
@@ -2885,7 +2886,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2894,7 +2895,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38">
         <v>41</v>
@@ -2911,7 +2912,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2920,7 +2921,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H39">
         <v>67</v>
@@ -2937,7 +2938,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2946,7 +2947,7 @@
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F40">
         <v>5.5</v>
@@ -2969,7 +2970,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2978,7 +2979,7 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F41">
         <v>12</v>
@@ -3001,7 +3002,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3010,7 +3011,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42">
         <v>7.5</v>
@@ -3033,7 +3034,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3042,7 +3043,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F43">
         <v>55</v>
@@ -3065,7 +3066,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3097,7 +3098,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3129,7 +3130,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3161,7 +3162,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3170,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F47">
         <v>5.4</v>
@@ -3193,7 +3194,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -3202,7 +3203,7 @@
         <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F48">
         <v>29.5</v>
@@ -3225,7 +3226,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -3234,7 +3235,7 @@
         <v>10</v>
       </c>
       <c r="E49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F49">
         <v>30</v>
@@ -3257,7 +3258,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>250</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3266,7 +3267,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F50">
         <v>12.5</v>
@@ -3289,7 +3290,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3298,7 +3299,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H51">
         <v>55</v>
@@ -3315,7 +3316,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3324,7 +3325,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H52">
         <v>100</v>
@@ -3341,7 +3342,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3350,7 +3351,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H53">
         <v>35</v>
@@ -3367,7 +3368,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3376,7 +3377,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H54">
         <v>60</v>
@@ -3393,7 +3394,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3402,7 +3403,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F55">
         <v>19.600000000000001</v>
@@ -3425,7 +3426,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3434,7 +3435,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F56">
         <v>76.599999999999994</v>
@@ -3457,7 +3458,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>251</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3466,7 +3467,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F57">
         <v>28</v>
@@ -3489,7 +3490,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3498,7 +3499,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F58">
         <v>32</v>
@@ -3521,7 +3522,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3530,7 +3531,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F59">
         <v>19</v>
@@ -3553,7 +3554,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3562,7 +3563,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F60">
         <v>155</v>
@@ -3585,7 +3586,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -3594,7 +3595,7 @@
         <v>10</v>
       </c>
       <c r="E61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F61">
         <v>12.4</v>
@@ -3617,7 +3618,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>278</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -3626,7 +3627,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F62">
         <v>20</v>
@@ -3649,7 +3650,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -3658,7 +3659,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F63">
         <v>54</v>
@@ -3681,7 +3682,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -3690,7 +3691,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F64">
         <v>19.5</v>
@@ -3713,7 +3714,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -3722,7 +3723,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F65">
         <v>56.5</v>
@@ -3745,7 +3746,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -3754,7 +3755,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F66">
         <v>48</v>
@@ -3777,7 +3778,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -3786,7 +3787,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F67">
         <v>19.5</v>
@@ -3809,7 +3810,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3818,7 +3819,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F68">
         <v>70.5</v>
@@ -3841,7 +3842,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3850,7 +3851,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F69">
         <v>130</v>
@@ -3873,7 +3874,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>252</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -3905,7 +3906,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3937,7 +3938,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -3969,7 +3970,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -3978,7 +3979,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F73">
         <v>45.5</v>
@@ -4001,7 +4002,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4010,7 +4011,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F74">
         <v>55</v>
@@ -4033,7 +4034,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4042,7 +4043,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H75">
         <v>80</v>
@@ -4059,7 +4060,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4068,7 +4069,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H76">
         <v>95</v>
@@ -4085,7 +4086,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4094,7 +4095,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H77">
         <v>120</v>
@@ -4111,7 +4112,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4120,7 +4121,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F78">
         <v>30</v>
@@ -4143,7 +4144,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4152,7 +4153,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F79">
         <v>95</v>
@@ -4175,7 +4176,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -4184,7 +4185,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F80">
         <v>36</v>
@@ -4207,7 +4208,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4216,7 +4217,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F81">
         <v>78.5</v>
@@ -4239,7 +4240,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4248,7 +4249,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F82">
         <v>6</v>
@@ -4271,7 +4272,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>254</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4280,7 +4281,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F83">
         <v>60</v>
@@ -4303,7 +4304,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -4312,7 +4313,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F84">
         <v>15</v>
@@ -4335,7 +4336,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -4344,7 +4345,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F85">
         <v>39.200000000000003</v>
@@ -4367,7 +4368,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -4376,7 +4377,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F86">
         <v>85.2</v>
@@ -4399,7 +4400,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -4408,7 +4409,7 @@
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F87">
         <v>90</v>
@@ -4431,7 +4432,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -4440,7 +4441,7 @@
         <v>10</v>
       </c>
       <c r="E88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F88">
         <v>120</v>
@@ -4463,7 +4464,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -4472,7 +4473,7 @@
         <v>10</v>
       </c>
       <c r="E89" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H89">
         <v>80</v>
@@ -4489,7 +4490,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -4498,7 +4499,7 @@
         <v>10</v>
       </c>
       <c r="E90" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H90">
         <v>105</v>
@@ -4515,7 +4516,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -4524,7 +4525,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F91">
         <v>4</v>
@@ -4547,7 +4548,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -4556,7 +4557,7 @@
         <v>10</v>
       </c>
       <c r="E92" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F92">
         <v>132.5</v>
@@ -4579,7 +4580,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -4588,7 +4589,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F93">
         <v>0.1</v>
@@ -4611,7 +4612,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -4620,7 +4621,7 @@
         <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F94">
         <v>0.1</v>
@@ -4643,7 +4644,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -4652,7 +4653,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F95">
         <v>40.5</v>
@@ -4675,7 +4676,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -4684,7 +4685,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F96">
         <v>210</v>
@@ -4707,7 +4708,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -4716,7 +4717,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F97">
         <v>32.4</v>
@@ -4739,7 +4740,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -4748,7 +4749,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F98">
         <v>75.599999999999994</v>
@@ -4771,7 +4772,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -4780,7 +4781,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F99">
         <v>6.5</v>
@@ -4803,7 +4804,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -4812,7 +4813,7 @@
         <v>10</v>
       </c>
       <c r="E100" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F100">
         <v>60</v>
@@ -4835,7 +4836,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -4844,7 +4845,7 @@
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F101">
         <v>10.4</v>
@@ -4867,7 +4868,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>121</v>
+        <v>255</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -4876,7 +4877,7 @@
         <v>10</v>
       </c>
       <c r="E102" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F102">
         <v>66.599999999999994</v>
@@ -4899,7 +4900,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -4931,7 +4932,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -4957,7 +4958,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -4966,7 +4967,7 @@
         <v>10</v>
       </c>
       <c r="E105" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F105">
         <v>6.5</v>
@@ -4989,7 +4990,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -4998,7 +4999,7 @@
         <v>10</v>
       </c>
       <c r="E106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H106">
         <v>80</v>
@@ -5015,7 +5016,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -5024,7 +5025,7 @@
         <v>10</v>
       </c>
       <c r="E107" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F107">
         <v>49.8</v>
@@ -5047,7 +5048,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -5056,7 +5057,7 @@
         <v>10</v>
       </c>
       <c r="E108" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F108">
         <v>50.2</v>
@@ -5079,7 +5080,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -5088,7 +5089,7 @@
         <v>10</v>
       </c>
       <c r="E109" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F109">
         <v>65.5</v>
@@ -5111,7 +5112,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -5120,7 +5121,7 @@
         <v>10</v>
       </c>
       <c r="E110" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -5143,7 +5144,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -5152,7 +5153,7 @@
         <v>10</v>
       </c>
       <c r="E111" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F111">
         <v>9.5</v>
@@ -5175,7 +5176,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -5184,7 +5185,7 @@
         <v>10</v>
       </c>
       <c r="E112" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F112">
         <v>115</v>
@@ -5207,7 +5208,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -5216,7 +5217,7 @@
         <v>10</v>
       </c>
       <c r="E113" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F113">
         <v>120</v>
@@ -5239,7 +5240,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -5248,7 +5249,7 @@
         <v>10</v>
       </c>
       <c r="E114" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F114">
         <v>34.6</v>
@@ -5271,7 +5272,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -5303,7 +5304,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -5312,7 +5313,7 @@
         <v>10</v>
       </c>
       <c r="E116" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F116">
         <v>80</v>
@@ -5335,7 +5336,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -5344,7 +5345,7 @@
         <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F117">
         <v>8</v>
@@ -5367,7 +5368,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>137</v>
+        <v>257</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -5376,7 +5377,7 @@
         <v>10</v>
       </c>
       <c r="E118" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F118">
         <v>25</v>
@@ -5399,7 +5400,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>276</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -5408,7 +5409,7 @@
         <v>10</v>
       </c>
       <c r="E119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F119">
         <v>15</v>
@@ -5431,7 +5432,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -5440,7 +5441,7 @@
         <v>10</v>
       </c>
       <c r="E120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F120">
         <v>39</v>
@@ -5463,7 +5464,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -5472,7 +5473,7 @@
         <v>10</v>
       </c>
       <c r="E121" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F121">
         <v>34.5</v>
@@ -5495,7 +5496,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -5504,7 +5505,7 @@
         <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F122">
         <v>80</v>
@@ -5527,7 +5528,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -5536,7 +5537,7 @@
         <v>10</v>
       </c>
       <c r="E123" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F123">
         <v>54.5</v>
@@ -5559,7 +5560,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>143</v>
+        <v>258</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -5568,7 +5569,7 @@
         <v>10</v>
       </c>
       <c r="E124" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F124">
         <v>56</v>
@@ -5591,7 +5592,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -5600,7 +5601,7 @@
         <v>10</v>
       </c>
       <c r="E125" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F125">
         <v>40.6</v>
@@ -5623,7 +5624,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>259</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -5632,7 +5633,7 @@
         <v>10</v>
       </c>
       <c r="E126" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F126">
         <v>30</v>
@@ -5655,7 +5656,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -5664,7 +5665,7 @@
         <v>10</v>
       </c>
       <c r="E127" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F127">
         <v>44.5</v>
@@ -5687,7 +5688,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -5696,7 +5697,7 @@
         <v>10</v>
       </c>
       <c r="E128" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F128">
         <v>55</v>
@@ -5719,7 +5720,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -5728,7 +5729,7 @@
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F129">
         <v>88.4</v>
@@ -5751,7 +5752,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -5760,7 +5761,7 @@
         <v>10</v>
       </c>
       <c r="E130" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F130">
         <v>10</v>
@@ -5783,7 +5784,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>151</v>
+        <v>260</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -5792,7 +5793,7 @@
         <v>10</v>
       </c>
       <c r="E131" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F131">
         <v>235</v>
@@ -5815,7 +5816,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -5824,7 +5825,7 @@
         <v>10</v>
       </c>
       <c r="E132" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F132">
         <v>220</v>
@@ -5847,7 +5848,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>153</v>
+        <v>261</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -5856,7 +5857,7 @@
         <v>10</v>
       </c>
       <c r="E133" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F133">
         <v>4</v>
@@ -5879,7 +5880,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>154</v>
+        <v>262</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -5888,7 +5889,7 @@
         <v>10</v>
       </c>
       <c r="E134" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F134">
         <v>6.5</v>
@@ -5911,7 +5912,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -5920,7 +5921,7 @@
         <v>10</v>
       </c>
       <c r="E135" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F135">
         <v>29</v>
@@ -5943,7 +5944,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -5952,7 +5953,7 @@
         <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F136">
         <v>24.5</v>
@@ -5975,7 +5976,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -5984,7 +5985,7 @@
         <v>10</v>
       </c>
       <c r="E137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F137">
         <v>25</v>
@@ -6007,7 +6008,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -6016,7 +6017,7 @@
         <v>10</v>
       </c>
       <c r="E138" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F138">
         <v>36.5</v>
@@ -6039,7 +6040,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -6048,7 +6049,7 @@
         <v>10</v>
       </c>
       <c r="E139" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F139">
         <v>7.5</v>
@@ -6071,7 +6072,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -6080,7 +6081,7 @@
         <v>10</v>
       </c>
       <c r="E140" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F140">
         <v>35</v>
@@ -6103,7 +6104,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -6112,7 +6113,7 @@
         <v>10</v>
       </c>
       <c r="E141" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F141">
         <v>11.5</v>
@@ -6135,7 +6136,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -6144,7 +6145,7 @@
         <v>10</v>
       </c>
       <c r="E142" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F142">
         <v>40.5</v>
@@ -6167,7 +6168,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>163</v>
+        <v>263</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -6176,7 +6177,7 @@
         <v>10</v>
       </c>
       <c r="E143" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F143">
         <v>59</v>
@@ -6199,7 +6200,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -6208,7 +6209,7 @@
         <v>10</v>
       </c>
       <c r="E144" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F144">
         <v>460</v>
@@ -6231,16 +6232,16 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E145" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F145">
         <v>55.4</v>
@@ -6263,16 +6264,16 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>167</v>
+        <v>264</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E146" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F146">
         <v>52.6</v>
@@ -6295,16 +6296,16 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E147" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F147">
         <v>60</v>
@@ -6327,7 +6328,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -6336,7 +6337,7 @@
         <v>10</v>
       </c>
       <c r="E148" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F148">
         <v>3.3</v>
@@ -6359,7 +6360,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -6368,7 +6369,7 @@
         <v>10</v>
       </c>
       <c r="E149" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F149">
         <v>16.5</v>
@@ -6391,7 +6392,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -6400,7 +6401,7 @@
         <v>10</v>
       </c>
       <c r="E150" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F150">
         <v>210</v>
@@ -6423,16 +6424,16 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E151" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F151">
         <v>122</v>
@@ -6455,16 +6456,16 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C152">
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E152" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F152">
         <v>4</v>
@@ -6487,7 +6488,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C153">
         <v>2</v>
@@ -6519,7 +6520,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C154">
         <v>2</v>
@@ -6551,7 +6552,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>177</v>
+        <v>265</v>
       </c>
       <c r="C155">
         <v>2</v>
@@ -6583,7 +6584,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>178</v>
+        <v>266</v>
       </c>
       <c r="C156">
         <v>2</v>
@@ -6592,7 +6593,7 @@
         <v>10</v>
       </c>
       <c r="E156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F156">
         <v>7.9</v>
@@ -6615,7 +6616,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C157">
         <v>2</v>
@@ -6624,7 +6625,7 @@
         <v>10</v>
       </c>
       <c r="E157" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F157">
         <v>19</v>
@@ -6647,7 +6648,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C158">
         <v>2</v>
@@ -6656,7 +6657,7 @@
         <v>10</v>
       </c>
       <c r="E158" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F158">
         <v>79.5</v>
@@ -6679,7 +6680,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C159">
         <v>2</v>
@@ -6688,7 +6689,7 @@
         <v>10</v>
       </c>
       <c r="E159" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F159">
         <v>9.5</v>
@@ -6711,7 +6712,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C160">
         <v>2</v>
@@ -6720,7 +6721,7 @@
         <v>10</v>
       </c>
       <c r="E160" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F160">
         <v>25</v>
@@ -6743,7 +6744,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="C161">
         <v>2</v>
@@ -6752,7 +6753,7 @@
         <v>10</v>
       </c>
       <c r="E161" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F161">
         <v>88.8</v>
@@ -6775,7 +6776,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="C162">
         <v>2</v>
@@ -6784,7 +6785,7 @@
         <v>10</v>
       </c>
       <c r="E162" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F162">
         <v>6</v>
@@ -6807,7 +6808,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="C163">
         <v>2</v>
@@ -6816,7 +6817,7 @@
         <v>10</v>
       </c>
       <c r="E163" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F163">
         <v>32.5</v>
@@ -6839,7 +6840,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="C164">
         <v>2</v>
@@ -6848,7 +6849,7 @@
         <v>10</v>
       </c>
       <c r="E164" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F164">
         <v>21.2</v>
@@ -6871,7 +6872,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="C165">
         <v>2</v>
@@ -6880,7 +6881,7 @@
         <v>10</v>
       </c>
       <c r="E165" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F165">
         <v>40.799999999999997</v>
@@ -6903,7 +6904,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="C166">
         <v>2</v>
@@ -6912,7 +6913,7 @@
         <v>10</v>
       </c>
       <c r="E166" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F166">
         <v>10.8</v>
@@ -6935,7 +6936,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="C167">
         <v>2</v>
@@ -6944,7 +6945,7 @@
         <v>10</v>
       </c>
       <c r="E167" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F167">
         <v>35.6</v>
@@ -6967,7 +6968,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="C168">
         <v>2</v>
@@ -6976,7 +6977,7 @@
         <v>10</v>
       </c>
       <c r="E168" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F168">
         <v>8.5</v>
@@ -6999,7 +7000,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="C169">
         <v>2</v>
@@ -7008,7 +7009,7 @@
         <v>10</v>
       </c>
       <c r="E169" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F169">
         <v>33.5</v>
@@ -7031,7 +7032,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="C170">
         <v>2</v>
@@ -7040,7 +7041,7 @@
         <v>10</v>
       </c>
       <c r="E170" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F170">
         <v>75</v>
@@ -7063,7 +7064,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="C171">
         <v>2</v>
@@ -7072,7 +7073,7 @@
         <v>10</v>
       </c>
       <c r="E171" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F171">
         <v>12</v>
@@ -7095,7 +7096,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="C172">
         <v>2</v>
@@ -7104,7 +7105,7 @@
         <v>10</v>
       </c>
       <c r="E172" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F172">
         <v>22.5</v>
@@ -7127,7 +7128,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="C173">
         <v>2</v>
@@ -7136,7 +7137,7 @@
         <v>10</v>
       </c>
       <c r="E173" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F173">
         <v>2</v>
@@ -7159,7 +7160,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>196</v>
+        <v>267</v>
       </c>
       <c r="C174">
         <v>2</v>
@@ -7168,7 +7169,7 @@
         <v>10</v>
       </c>
       <c r="E174" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F174">
         <v>3</v>
@@ -7191,7 +7192,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C175">
         <v>2</v>
@@ -7200,7 +7201,7 @@
         <v>10</v>
       </c>
       <c r="E175" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F175">
         <v>1</v>
@@ -7223,7 +7224,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="C176">
         <v>2</v>
@@ -7232,7 +7233,7 @@
         <v>10</v>
       </c>
       <c r="E176" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F176">
         <v>1.5</v>
@@ -7255,7 +7256,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="C177">
         <v>2</v>
@@ -7264,7 +7265,7 @@
         <v>10</v>
       </c>
       <c r="E177" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F177">
         <v>3.2</v>
@@ -7287,7 +7288,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C178">
         <v>2</v>
@@ -7296,7 +7297,7 @@
         <v>10</v>
       </c>
       <c r="E178" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F178">
         <v>2</v>
@@ -7319,7 +7320,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="C179">
         <v>2</v>
@@ -7328,7 +7329,7 @@
         <v>10</v>
       </c>
       <c r="E179" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F179">
         <v>15</v>
@@ -7351,7 +7352,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="C180">
         <v>2</v>
@@ -7360,7 +7361,7 @@
         <v>10</v>
       </c>
       <c r="E180" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F180">
         <v>7.8</v>
@@ -7383,7 +7384,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="C181">
         <v>2</v>
@@ -7392,7 +7393,7 @@
         <v>10</v>
       </c>
       <c r="E181" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F181">
         <v>13.3</v>
@@ -7415,7 +7416,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="C182">
         <v>2</v>
@@ -7424,7 +7425,7 @@
         <v>10</v>
       </c>
       <c r="E182" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F182">
         <v>61.5</v>
@@ -7447,7 +7448,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="C183">
         <v>2</v>
@@ -7479,7 +7480,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="C184">
         <v>2</v>
@@ -7488,7 +7489,7 @@
         <v>10</v>
       </c>
       <c r="E184" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F184">
         <v>8.5</v>
@@ -7511,7 +7512,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C185">
         <v>2</v>
@@ -7520,7 +7521,7 @@
         <v>10</v>
       </c>
       <c r="E185" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F185">
         <v>28.5</v>
@@ -7543,7 +7544,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="C186">
         <v>2</v>
@@ -7552,7 +7553,7 @@
         <v>10</v>
       </c>
       <c r="E186" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F186">
         <v>38</v>
@@ -7575,7 +7576,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C187">
         <v>2</v>
@@ -7584,7 +7585,7 @@
         <v>10</v>
       </c>
       <c r="E187" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F187">
         <v>33.9</v>
@@ -7607,7 +7608,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="C188">
         <v>2</v>
@@ -7639,7 +7640,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C189">
         <v>2</v>
@@ -7671,7 +7672,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="C190">
         <v>2</v>
@@ -7703,7 +7704,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="C191">
         <v>2</v>
@@ -7712,7 +7713,7 @@
         <v>10</v>
       </c>
       <c r="E191" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F191">
         <v>11.5</v>
@@ -7735,7 +7736,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="C192">
         <v>2</v>
@@ -7767,7 +7768,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="C193">
         <v>2</v>
@@ -7799,7 +7800,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="C194">
         <v>2</v>
@@ -7808,7 +7809,7 @@
         <v>10</v>
       </c>
       <c r="E194" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F194">
         <v>38</v>
@@ -7831,7 +7832,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="C195">
         <v>2</v>
@@ -7840,7 +7841,7 @@
         <v>10</v>
       </c>
       <c r="E195" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F195">
         <v>8.5</v>
@@ -7863,7 +7864,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="C196">
         <v>2</v>
@@ -7872,7 +7873,7 @@
         <v>10</v>
       </c>
       <c r="E196" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F196">
         <v>75</v>
@@ -7895,7 +7896,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="C197">
         <v>2</v>
@@ -7904,7 +7905,7 @@
         <v>10</v>
       </c>
       <c r="E197" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F197">
         <v>26.5</v>
@@ -7927,7 +7928,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C198">
         <v>2</v>
@@ -7936,7 +7937,7 @@
         <v>10</v>
       </c>
       <c r="E198" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F198">
         <v>27</v>
@@ -7959,7 +7960,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>222</v>
+        <v>277</v>
       </c>
       <c r="C199">
         <v>2</v>
@@ -7968,7 +7969,7 @@
         <v>10</v>
       </c>
       <c r="E199" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F199">
         <v>2.1</v>
@@ -7991,7 +7992,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="C200">
         <v>2</v>
@@ -8000,7 +8001,7 @@
         <v>10</v>
       </c>
       <c r="E200" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F200">
         <v>79.5</v>
@@ -8023,7 +8024,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>224</v>
+        <v>279</v>
       </c>
       <c r="C201">
         <v>2</v>
@@ -8032,7 +8033,7 @@
         <v>10</v>
       </c>
       <c r="E201" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F201">
         <v>1</v>
@@ -8055,7 +8056,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C202">
         <v>2</v>
@@ -8064,7 +8065,7 @@
         <v>10</v>
       </c>
       <c r="E202" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F202">
         <v>5</v>
@@ -8087,7 +8088,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>226</v>
+        <v>269</v>
       </c>
       <c r="C203">
         <v>2</v>
@@ -8096,7 +8097,7 @@
         <v>10</v>
       </c>
       <c r="E203" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F203">
         <v>28.5</v>
@@ -8119,7 +8120,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="C204">
         <v>2</v>
@@ -8128,7 +8129,7 @@
         <v>10</v>
       </c>
       <c r="E204" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F204">
         <v>41.5</v>
@@ -8151,7 +8152,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
       <c r="C205">
         <v>2</v>
@@ -8160,7 +8161,7 @@
         <v>10</v>
       </c>
       <c r="E205" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F205">
         <v>7.2</v>
@@ -8183,7 +8184,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
       <c r="C206">
         <v>2</v>
@@ -8192,7 +8193,7 @@
         <v>10</v>
       </c>
       <c r="E206" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F206">
         <v>125.8</v>
@@ -8215,7 +8216,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="C207">
         <v>2</v>
@@ -8224,7 +8225,7 @@
         <v>10</v>
       </c>
       <c r="E207" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F207">
         <v>14</v>
@@ -8247,7 +8248,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="C208">
         <v>2</v>
@@ -8256,7 +8257,7 @@
         <v>10</v>
       </c>
       <c r="E208" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F208">
         <v>64.8</v>
@@ -8279,7 +8280,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="C209">
         <v>2</v>
@@ -8288,7 +8289,7 @@
         <v>10</v>
       </c>
       <c r="E209" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="F209">
         <v>400</v>
@@ -8311,7 +8312,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
       <c r="C210">
         <v>2</v>
@@ -8320,7 +8321,7 @@
         <v>10</v>
       </c>
       <c r="E210" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F210">
         <v>7.8</v>
@@ -8343,7 +8344,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="C211">
         <v>2</v>
@@ -8352,7 +8353,7 @@
         <v>10</v>
       </c>
       <c r="E211" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F211">
         <v>48.7</v>
@@ -8375,7 +8376,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="C212">
         <v>2</v>
@@ -8384,7 +8385,7 @@
         <v>10</v>
       </c>
       <c r="E212" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F212">
         <v>3.9</v>
@@ -8407,7 +8408,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="C213">
         <v>2</v>
@@ -8416,7 +8417,7 @@
         <v>10</v>
       </c>
       <c r="E213" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F213">
         <v>118</v>
@@ -8439,7 +8440,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="C214">
         <v>2</v>
@@ -8448,7 +8449,7 @@
         <v>10</v>
       </c>
       <c r="E214" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F214">
         <v>20.5</v>
@@ -8471,7 +8472,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="C215">
         <v>2</v>
@@ -8480,7 +8481,7 @@
         <v>10</v>
       </c>
       <c r="E215" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F215">
         <v>54</v>
@@ -8503,7 +8504,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="C216">
         <v>2</v>
@@ -8512,7 +8513,7 @@
         <v>10</v>
       </c>
       <c r="E216" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F216">
         <v>28</v>
@@ -8535,7 +8536,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="C217">
         <v>2</v>
@@ -8544,7 +8545,7 @@
         <v>10</v>
       </c>
       <c r="E217" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F217">
         <v>8.8000000000000007</v>
@@ -8567,7 +8568,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="C218">
         <v>2</v>
@@ -8576,7 +8577,7 @@
         <v>10</v>
       </c>
       <c r="E218" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F218">
         <v>125.8</v>
@@ -8599,7 +8600,7 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="C219">
         <v>2</v>
@@ -8608,7 +8609,7 @@
         <v>10</v>
       </c>
       <c r="E219" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F219">
         <v>35</v>
@@ -8631,7 +8632,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="C220">
         <v>2</v>
@@ -8640,7 +8641,7 @@
         <v>10</v>
       </c>
       <c r="E220" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F220">
         <v>55</v>
@@ -8663,7 +8664,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="C221">
         <v>2</v>
@@ -8672,7 +8673,7 @@
         <v>10</v>
       </c>
       <c r="E221" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F221">
         <v>6.5</v>
@@ -8695,7 +8696,7 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="C222">
         <v>2</v>
@@ -8704,7 +8705,7 @@
         <v>10</v>
       </c>
       <c r="E222" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F222">
         <v>55.8</v>
@@ -8727,7 +8728,7 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="C223">
         <v>2</v>
@@ -8736,7 +8737,7 @@
         <v>10</v>
       </c>
       <c r="E223" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F223">
         <v>5</v>
@@ -8759,7 +8760,7 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="C224">
         <v>2</v>
@@ -8768,7 +8769,7 @@
         <v>10</v>
       </c>
       <c r="E224" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F224">
         <v>12</v>
@@ -8791,7 +8792,7 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="C225">
         <v>2</v>
@@ -8800,7 +8801,7 @@
         <v>10</v>
       </c>
       <c r="E225" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F225">
         <v>28.5</v>
@@ -8823,7 +8824,7 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="C226">
         <v>2</v>
@@ -8832,7 +8833,7 @@
         <v>10</v>
       </c>
       <c r="E226" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F226">
         <v>16</v>
@@ -8855,7 +8856,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C227">
         <v>2</v>
@@ -8864,7 +8865,7 @@
         <v>10</v>
       </c>
       <c r="E227" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F227">
         <v>220</v>
@@ -8887,7 +8888,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="C228">
         <v>2</v>
@@ -8896,7 +8897,7 @@
         <v>10</v>
       </c>
       <c r="E228" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="F228">
         <v>50.5</v>
@@ -8919,7 +8920,7 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="C229">
         <v>2</v>
@@ -8928,7 +8929,7 @@
         <v>10</v>
       </c>
       <c r="E229" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F229">
         <v>10.8</v>
@@ -8951,7 +8952,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="C230">
         <v>2</v>
@@ -8960,7 +8961,7 @@
         <v>10</v>
       </c>
       <c r="E230" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F230">
         <v>35</v>
@@ -8983,7 +8984,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="C231">
         <v>2</v>
@@ -8992,7 +8993,7 @@
         <v>10</v>
       </c>
       <c r="E231" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F231">
         <v>152</v>
@@ -9015,7 +9016,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="C232">
         <v>2</v>
@@ -9024,7 +9025,7 @@
         <v>10</v>
       </c>
       <c r="E232" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F232">
         <v>33.5</v>
@@ -9047,7 +9048,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="C233">
         <v>2</v>
@@ -9056,7 +9057,7 @@
         <v>10</v>
       </c>
       <c r="E233" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F233">
         <v>120</v>
@@ -9079,7 +9080,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="C234">
         <v>2</v>
@@ -9088,7 +9089,7 @@
         <v>10</v>
       </c>
       <c r="E234" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F234">
         <v>32.5</v>
@@ -9111,7 +9112,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="C235">
         <v>2</v>
@@ -9120,7 +9121,7 @@
         <v>10</v>
       </c>
       <c r="E235" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F235">
         <v>71.2</v>
@@ -9143,7 +9144,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="C236">
         <v>2</v>
@@ -9152,7 +9153,7 @@
         <v>10</v>
       </c>
       <c r="E236" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F236">
         <v>58</v>
@@ -9175,7 +9176,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="C237">
         <v>2</v>
@@ -9184,7 +9185,7 @@
         <v>10</v>
       </c>
       <c r="E237" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F237">
         <v>21</v>
@@ -9207,7 +9208,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="C238">
         <v>2</v>
@@ -9216,7 +9217,7 @@
         <v>10</v>
       </c>
       <c r="E238" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F238">
         <v>48</v>
@@ -9239,7 +9240,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="C239">
         <v>2</v>
@@ -9248,7 +9249,7 @@
         <v>10</v>
       </c>
       <c r="E239" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F239">
         <v>6</v>
@@ -9271,7 +9272,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="C240">
         <v>2</v>
@@ -9280,7 +9281,7 @@
         <v>10</v>
       </c>
       <c r="E240" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F240">
         <v>23.5</v>
@@ -9303,7 +9304,7 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>265</v>
+        <v>234</v>
       </c>
       <c r="C241">
         <v>2</v>
@@ -9312,7 +9313,7 @@
         <v>10</v>
       </c>
       <c r="E241" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F241">
         <v>21.4</v>
@@ -9335,7 +9336,7 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C242">
         <v>2</v>
@@ -9344,7 +9345,7 @@
         <v>10</v>
       </c>
       <c r="E242" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F242">
         <v>75.5</v>
@@ -9367,7 +9368,7 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
       <c r="C243">
         <v>2</v>
@@ -9376,7 +9377,7 @@
         <v>10</v>
       </c>
       <c r="E243" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F243">
         <v>46.8</v>
@@ -9399,16 +9400,16 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
       <c r="C244">
         <v>2</v>
       </c>
       <c r="D244" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E244" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F244">
         <v>178</v>
@@ -9431,16 +9432,16 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="C245">
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E245" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F245">
         <v>198</v>
@@ -9463,16 +9464,16 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="C246">
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E246" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F246">
         <v>187</v>
@@ -9495,7 +9496,7 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="C247">
         <v>2</v>
@@ -9504,7 +9505,7 @@
         <v>10</v>
       </c>
       <c r="E247" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F247">
         <v>72</v>
@@ -9527,7 +9528,7 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="C248">
         <v>2</v>
@@ -9536,7 +9537,7 @@
         <v>10</v>
       </c>
       <c r="E248" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F248">
         <v>152</v>
@@ -9559,7 +9560,7 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="C249">
         <v>2</v>
@@ -9568,7 +9569,7 @@
         <v>10</v>
       </c>
       <c r="E249" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F249">
         <v>202</v>
@@ -9591,16 +9592,16 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="C250">
         <v>2</v>
       </c>
       <c r="D250" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E250" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F250">
         <v>216</v>
@@ -9623,16 +9624,16 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="C251">
         <v>2</v>
       </c>
       <c r="D251" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E251" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F251">
         <v>199</v>
@@ -9655,16 +9656,16 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="C252">
         <v>2</v>
       </c>
       <c r="D252" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E252" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F252">
         <v>5</v>

</xml_diff>